<commit_message>
done 4 exrcises from w6d1 update
</commit_message>
<xml_diff>
--- a/Week6/Day1/ExerciseXP/WrongMove(ex4).xlsx
+++ b/Week6/Day1/ExerciseXP/WrongMove(ex4).xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margotiamanova/Desktop/DI-Bootcamp/Week6/Day1/ExerciseXP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1075337C-2587-F94F-9582-AB2392FB227C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374790D1-CFC4-6942-97D4-581F33AD3797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
     <sheet name="Properties" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="31" r:id="rId3"/>
+    <pivotCache cacheId="13" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="81">
   <si>
     <t>PostCode</t>
   </si>
@@ -271,25 +271,16 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Sum of Field1</t>
-  </si>
-  <si>
     <t>Sum of Total Rooms</t>
   </si>
   <si>
-    <t>Column Labels</t>
-  </si>
-  <si>
-    <t>Total Sum of Field1</t>
-  </si>
-  <si>
-    <t>Total Sum of Total Rooms</t>
-  </si>
-  <si>
     <t>Group1</t>
   </si>
   <si>
-    <t>Group1 Total</t>
+    <t>Group2</t>
+  </si>
+  <si>
+    <t>Count of Garden Size</t>
   </si>
 </sst>
 </file>
@@ -366,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -399,9 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -421,16 +409,72 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45732.718198263887" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="56" xr:uid="{D09D0692-0969-704A-9549-C60BC2ECCA0B}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45732.821695833336" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="56" xr:uid="{CB83F0DC-982A-0C45-AABE-67A8051A5ADA}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A3:K59" sheet="Properties"/>
   </cacheSource>
-  <cacheFields count="14">
+  <cacheFields count="13">
     <cacheField name="PostCode" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="49">
+        <s v="SK13 7AZ"/>
+        <s v="SK22 9GT"/>
+        <s v="SK13 6DD"/>
+        <s v="SK14 8DS"/>
+        <s v="SK13 7CW"/>
+        <s v="SK22 3YT"/>
+        <s v="SK13 4DF"/>
+        <s v="SK14 7AD"/>
+        <s v="SK13 2AA"/>
+        <s v="SK13 5YY"/>
+        <s v="SK14 9FT"/>
+        <s v="SK23 4RF"/>
+        <s v="SK13 1GG"/>
+        <s v="SK13 6YH"/>
+        <s v="SK22 8BN"/>
+        <s v="SK14 7JJ"/>
+        <s v="SK22 3LP"/>
+        <s v="SK13 4DT"/>
+        <s v="SK13 9SS"/>
+        <s v="SK14 6HN"/>
+        <s v="SK23 3KM"/>
+        <s v="SK23 5WW"/>
+        <s v="SK13 8FS"/>
+        <s v="SK13 4RL"/>
+        <s v="SK14 7YT"/>
+        <s v="SK13 5EE"/>
+        <s v="SK23 4VS"/>
+        <s v="SK16 8NV"/>
+        <s v="SK14 3DD"/>
+        <s v="SK13 4DE"/>
+        <s v="SK13 6LK"/>
+        <s v="SK13 9PF"/>
+        <s v="SK14 8BM"/>
+        <s v="SK14 6DH"/>
+        <s v="SK13 3SS"/>
+        <s v="SK13 4AK"/>
+        <s v="SK13 4XC"/>
+        <s v="SK14 6RL"/>
+        <s v="SK13 7PJ"/>
+        <s v="SK13 6FD"/>
+        <s v="SK14 3FD"/>
+        <s v="SK13 2WD"/>
+        <s v="SK22 1XV"/>
+        <s v="SK13 5LS"/>
+        <s v="SK13 6HH"/>
+        <s v="SK14 8GP"/>
+        <s v="SK15 6YW"/>
+        <s v="SK13 4DD"/>
+        <s v="SK13 4RF"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="5">
+        <s v="Detatched"/>
+        <s v="Semi-detatched"/>
+        <s v="Terraced"/>
+        <s v="Bungalow"/>
+        <s v="Flat"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Location" numFmtId="0">
       <sharedItems count="4">
@@ -439,33 +483,24 @@
         <s v="Countryside"/>
         <s v="Remote"/>
       </sharedItems>
-      <fieldGroup par="13"/>
+      <fieldGroup par="12"/>
     </cacheField>
     <cacheField name="Bedrooms" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5" count="5">
-        <n v="4"/>
-        <n v="3"/>
-        <n v="2"/>
-        <n v="1"/>
-        <n v="5"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
     </cacheField>
     <cacheField name="Bathrooms" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="3" count="3">
-        <n v="2"/>
-        <n v="1"/>
-        <n v="3"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="3"/>
     </cacheField>
     <cacheField name="Reception Rooms" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="3" count="3">
-        <n v="3"/>
-        <n v="2"/>
-        <n v="1"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="3"/>
     </cacheField>
     <cacheField name="Garden Size" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="4">
+        <s v="Medium"/>
+        <s v="Small"/>
+        <s v="Large"/>
+        <s v="None"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Date on Market" numFmtId="14">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2021-06-05T00:00:00" maxDate="2022-10-18T00:00:00"/>
@@ -479,18 +514,18 @@
     <cacheField name="Sale Price" numFmtId="164">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="158500" maxValue="495000"/>
     </cacheField>
-    <cacheField name="Field1" numFmtId="0" formula=" 0" databaseField="0"/>
     <cacheField name="Total Rooms" numFmtId="0" formula="Bedrooms +Bathrooms +'Reception Rooms'" databaseField="0"/>
     <cacheField name="Location2" numFmtId="0" databaseField="0">
       <fieldGroup base="2">
         <discretePr count="4">
-          <x v="0"/>
-          <x v="0"/>
+          <x v="1"/>
+          <x v="1"/>
           <x v="0"/>
           <x v="0"/>
         </discretePr>
-        <groupItems count="1">
+        <groupItems count="2">
           <s v="Group1"/>
+          <s v="Group2"/>
         </groupItems>
       </fieldGroup>
     </cacheField>
@@ -506,728 +541,728 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="56">
   <r>
-    <s v="SK13 7AZ"/>
-    <s v="Detatched"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Medium"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <x v="0"/>
     <d v="2021-11-25T00:00:00"/>
     <m/>
     <n v="345000"/>
     <m/>
   </r>
   <r>
-    <s v="SK22 9GT"/>
-    <s v="Semi-detatched"/>
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
     <x v="1"/>
-    <s v="Small"/>
     <d v="2021-07-17T00:00:00"/>
     <d v="2022-01-31T00:00:00"/>
     <n v="245000"/>
     <n v="238500"/>
   </r>
   <r>
-    <s v="SK13 6DD"/>
-    <s v="Terraced"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
     <x v="1"/>
-    <x v="1"/>
-    <s v="Small"/>
     <d v="2021-10-23T00:00:00"/>
     <d v="2021-12-18T00:00:00"/>
     <n v="199000"/>
     <n v="199000"/>
   </r>
   <r>
-    <s v="SK14 8DS"/>
-    <s v="Detatched"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2022-10-17T00:00:00"/>
     <d v="2022-01-22T00:00:00"/>
     <n v="398000"/>
     <n v="387500"/>
   </r>
   <r>
-    <s v="SK13 7CW"/>
-    <s v="Semi-detatched"/>
-    <x v="0"/>
+    <x v="4"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-11-28T00:00:00"/>
     <d v="2022-12-18T00:00:00"/>
     <n v="329000"/>
     <n v="319500"/>
   </r>
   <r>
-    <s v="SK22 3YT"/>
-    <s v="Detatched"/>
+    <x v="5"/>
+    <x v="0"/>
     <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Large"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <x v="2"/>
     <d v="2021-10-12T00:00:00"/>
     <m/>
     <n v="478500"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 4DF"/>
-    <s v="Terraced"/>
-    <x v="0"/>
-    <x v="2"/>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
     <x v="1"/>
-    <x v="1"/>
-    <s v="Small"/>
     <d v="2021-09-04T00:00:00"/>
     <d v="2021-01-15T00:00:00"/>
     <n v="213000"/>
     <n v="199500"/>
   </r>
   <r>
-    <s v="SK14 7AD"/>
-    <s v="Semi-detatched"/>
-    <x v="0"/>
+    <x v="7"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-10-28T00:00:00"/>
     <d v="2022-02-17T00:00:00"/>
     <n v="278500"/>
     <n v="277000"/>
   </r>
   <r>
-    <s v="SK13 2AA"/>
-    <s v="Semi-detatched"/>
+    <x v="8"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-08-10T00:00:00"/>
     <m/>
     <n v="278500"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 5YY"/>
-    <s v="Terraced"/>
-    <x v="0"/>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Small"/>
     <d v="2021-10-29T00:00:00"/>
     <d v="2022-01-28T00:00:00"/>
     <n v="176500"/>
     <n v="174300"/>
   </r>
   <r>
-    <s v="SK14 9FT"/>
-    <s v="Bungalow"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-11-15T00:00:00"/>
     <d v="2022-01-12T00:00:00"/>
     <n v="223750"/>
     <n v="219750"/>
   </r>
   <r>
-    <s v="SK23 4RF"/>
-    <s v="Flat"/>
-    <x v="0"/>
+    <x v="11"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
     <x v="3"/>
-    <x v="1"/>
-    <x v="2"/>
-    <s v="None"/>
     <d v="2021-11-14T00:00:00"/>
     <m/>
     <n v="135000"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 1GG"/>
-    <s v="Terraced"/>
-    <x v="0"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="Small"/>
     <d v="2022-01-04T00:00:00"/>
     <d v="2022-01-18T00:00:00"/>
     <n v="165900"/>
     <n v="168000"/>
   </r>
   <r>
-    <s v="SK13 6YH"/>
-    <s v="Bungalow"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="13"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-09-14T00:00:00"/>
     <d v="2021-12-27T00:00:00"/>
     <n v="415500"/>
     <n v="419500"/>
   </r>
   <r>
-    <s v="SK13 6YH"/>
-    <s v="Bungalow"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="13"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-09-14T00:00:00"/>
     <d v="2021-12-27T00:00:00"/>
     <n v="415500"/>
     <n v="419500"/>
   </r>
   <r>
-    <s v="SK13 6YH"/>
-    <s v="Bungalow"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="13"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-09-14T00:00:00"/>
     <d v="2021-12-27T00:00:00"/>
     <n v="415500"/>
     <n v="419500"/>
   </r>
   <r>
-    <s v="SK13 6YH"/>
-    <s v="Bungalow"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="13"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-09-10T00:00:00"/>
     <d v="1903-12-30T00:00:00"/>
     <n v="199500"/>
     <m/>
   </r>
   <r>
-    <s v="SK22 8BN"/>
-    <s v="Flat"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <s v="None"/>
+    <x v="14"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="3"/>
     <d v="2021-10-02T00:00:00"/>
     <d v="2022-01-18T00:00:00"/>
     <n v="175500"/>
     <n v="169500"/>
   </r>
   <r>
-    <s v="SK14 7JJ"/>
-    <s v="Semi-detatched"/>
-    <x v="2"/>
+    <x v="15"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-12-20T00:00:00"/>
     <d v="2022-02-14T00:00:00"/>
     <n v="319750"/>
     <n v="315750"/>
   </r>
   <r>
-    <s v="SK22 3LP"/>
-    <s v="Bungalow"/>
+    <x v="16"/>
     <x v="3"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="3"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-10-14T00:00:00"/>
     <m/>
     <n v="289500"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 4DT"/>
-    <s v="Detatched"/>
-    <x v="2"/>
-    <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Large"/>
+    <x v="17"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <x v="2"/>
     <d v="2021-08-08T00:00:00"/>
     <m/>
     <n v="525750"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 9SS"/>
-    <s v="Detatched"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="18"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-11-13T00:00:00"/>
     <d v="2022-02-24T00:00:00"/>
     <n v="495000"/>
     <n v="495000"/>
   </r>
   <r>
-    <s v="SK14 6HN"/>
-    <s v="Semi-detatched"/>
-    <x v="0"/>
+    <x v="19"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-08-05T00:00:00"/>
     <d v="2022-01-14T00:00:00"/>
     <n v="369500"/>
     <n v="362500"/>
   </r>
   <r>
-    <s v="SK14 6HN"/>
-    <s v="Semi-detatched"/>
+    <x v="19"/>
+    <x v="1"/>
     <x v="3"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Small"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <x v="1"/>
     <d v="2022-01-03T00:00:00"/>
     <d v="1903-12-30T00:00:00"/>
     <n v="176500"/>
     <m/>
   </r>
   <r>
-    <s v="SK23 3KM"/>
-    <s v="Terraced"/>
+    <x v="20"/>
+    <x v="2"/>
     <x v="3"/>
-    <x v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
     <x v="1"/>
-    <x v="2"/>
-    <s v="Small"/>
     <d v="2021-09-01T00:00:00"/>
     <m/>
     <n v="142500"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 6YH"/>
-    <s v="Bungalow"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="13"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-09-14T00:00:00"/>
     <d v="2021-12-27T00:00:00"/>
     <n v="415500"/>
     <n v="419500"/>
   </r>
   <r>
-    <s v="SK23 5WW"/>
-    <s v="Bungalow"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="21"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-10-16T00:00:00"/>
     <d v="2022-02-12T00:00:00"/>
     <n v="314250"/>
     <n v="309750"/>
   </r>
   <r>
-    <s v="SK13 8FS"/>
-    <s v="Terraced"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="22"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
     <x v="1"/>
-    <x v="2"/>
-    <s v="Small"/>
     <d v="2021-08-22T00:00:00"/>
     <m/>
     <n v="178500"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 4RL"/>
-    <s v="Semi-detatched"/>
-    <x v="0"/>
+    <x v="23"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2022-01-10T00:00:00"/>
     <d v="2022-02-24T00:00:00"/>
     <n v="305000"/>
     <n v="302750"/>
   </r>
   <r>
-    <s v="SK14 7YT"/>
-    <s v="Detatched"/>
+    <x v="24"/>
+    <x v="0"/>
     <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-10-30T00:00:00"/>
     <d v="2022-02-14T00:00:00"/>
     <n v="435000"/>
     <n v="429500"/>
   </r>
   <r>
-    <s v="SK13 5EE"/>
-    <s v="Semi-detatched"/>
-    <x v="2"/>
+    <x v="25"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Medium"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <x v="0"/>
     <d v="2021-09-10T00:00:00"/>
     <d v="2022-02-14T00:00:00"/>
     <n v="385000"/>
     <n v="375500"/>
   </r>
   <r>
-    <s v="SK23 4VS"/>
-    <s v="Detatched"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="26"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-09-04T00:00:00"/>
     <d v="2021-10-16T00:00:00"/>
     <n v="405000"/>
     <n v="405000"/>
   </r>
   <r>
-    <s v="SK16 8NV"/>
-    <s v="Terraced"/>
-    <x v="0"/>
-    <x v="2"/>
+    <x v="27"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
     <x v="1"/>
-    <x v="2"/>
-    <s v="Small"/>
     <d v="2021-08-01T00:00:00"/>
     <d v="2021-11-29T00:00:00"/>
     <n v="159000"/>
     <n v="158500"/>
   </r>
   <r>
-    <s v="SK14 3DD"/>
-    <s v="Semi-detatched"/>
-    <x v="0"/>
+    <x v="28"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-08-05T00:00:00"/>
     <d v="2021-12-10T00:00:00"/>
     <n v="278000"/>
     <n v="276500"/>
   </r>
   <r>
-    <s v="SK13 4DE"/>
-    <s v="Terraced"/>
-    <x v="0"/>
-    <x v="2"/>
+    <x v="29"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
     <x v="1"/>
-    <x v="2"/>
-    <s v="Small"/>
     <d v="2021-07-02T00:00:00"/>
     <d v="2022-02-24T00:00:00"/>
     <n v="178600"/>
     <n v="175500"/>
   </r>
   <r>
-    <s v="SK13 6LK"/>
-    <s v="Detatched"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="30"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-08-23T00:00:00"/>
     <d v="2022-01-16T00:00:00"/>
     <n v="435000"/>
     <n v="431750"/>
   </r>
   <r>
-    <s v="SK13 9PF"/>
-    <s v="Semi-detatched"/>
-    <x v="2"/>
+    <x v="31"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-07-18T00:00:00"/>
     <d v="2021-12-10T00:00:00"/>
     <n v="345500"/>
     <n v="342500"/>
   </r>
   <r>
-    <s v="SK14 8BM"/>
-    <s v="Detatched"/>
+    <x v="32"/>
+    <x v="0"/>
     <x v="3"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-08-22T00:00:00"/>
     <d v="2021-12-18T00:00:00"/>
     <n v="418500"/>
     <n v="422500"/>
   </r>
   <r>
-    <s v="SK14 6DH"/>
-    <s v="Semi-detatched"/>
-    <x v="2"/>
+    <x v="33"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-11-15T00:00:00"/>
     <m/>
     <n v="375500"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 3SS"/>
-    <s v="Terraced"/>
-    <x v="0"/>
-    <x v="2"/>
+    <x v="34"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
     <x v="1"/>
-    <x v="2"/>
-    <s v="Small"/>
     <d v="2021-10-02T00:00:00"/>
     <m/>
     <n v="169500"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 6YH"/>
-    <s v="Bungalow"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="13"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-09-14T00:00:00"/>
     <d v="2021-12-27T00:00:00"/>
     <n v="415500"/>
     <n v="419500"/>
   </r>
   <r>
-    <s v="SK13 4AK"/>
-    <s v="Bungalow"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="35"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-08-14T00:00:00"/>
     <d v="2022-01-26T00:00:00"/>
     <n v="298500"/>
     <n v="298500"/>
   </r>
   <r>
-    <s v="SK13 4XC"/>
-    <s v="Semi-detatched"/>
-    <x v="2"/>
+    <x v="36"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-07-10T00:00:00"/>
     <d v="2022-01-21T00:00:00"/>
     <n v="331750"/>
     <n v="330500"/>
   </r>
   <r>
-    <s v="SK14 6RL"/>
-    <s v="Detatched"/>
+    <x v="37"/>
+    <x v="0"/>
     <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-08-02T00:00:00"/>
     <d v="2021-12-10T00:00:00"/>
     <n v="385500"/>
     <n v="383500"/>
   </r>
   <r>
-    <s v="SK13 7PJ"/>
-    <s v="Semi-detatched"/>
-    <x v="2"/>
+    <x v="38"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-09-25T00:00:00"/>
     <d v="2022-02-02T00:00:00"/>
     <n v="322500"/>
     <n v="319500"/>
   </r>
   <r>
-    <s v="SK13 6FD"/>
-    <s v="Semi-detatched"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Medium"/>
+    <x v="39"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <x v="0"/>
     <d v="2021-08-04T00:00:00"/>
     <d v="2021-11-15T00:00:00"/>
     <n v="365500"/>
     <n v="365500"/>
   </r>
   <r>
-    <s v="SK14 3FD"/>
-    <s v="Detatched"/>
-    <x v="0"/>
+    <x v="40"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="Small"/>
     <d v="2021-07-13T00:00:00"/>
     <m/>
     <n v="312750"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 2WD"/>
-    <s v="Detatched"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <x v="41"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-06-23T00:00:00"/>
     <d v="2022-01-03T00:00:00"/>
     <n v="309500"/>
     <n v="304500"/>
   </r>
   <r>
-    <s v="SK22 1XV"/>
-    <s v="Terraced"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="42"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
     <x v="1"/>
-    <x v="2"/>
-    <s v="Small"/>
     <d v="2021-10-14T00:00:00"/>
     <d v="2022-02-04T00:00:00"/>
     <n v="204500"/>
     <n v="203900"/>
   </r>
   <r>
-    <s v="SK13 5LS"/>
-    <s v="Semi-detatched"/>
-    <x v="0"/>
+    <x v="43"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
-    <s v="Medium"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-07-03T00:00:00"/>
     <m/>
     <n v="225500"/>
     <m/>
   </r>
   <r>
-    <s v="SK13 6YH"/>
-    <s v="Bungalow"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="13"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-09-14T00:00:00"/>
     <d v="2021-12-27T00:00:00"/>
     <n v="415500"/>
     <n v="419500"/>
   </r>
   <r>
-    <s v="SK13 6HH"/>
-    <s v="Semi-detatched"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="44"/>
     <x v="1"/>
-    <s v="Medium"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
     <d v="2021-08-31T00:00:00"/>
     <d v="2021-10-04T00:00:00"/>
     <n v="209500"/>
     <n v="209500"/>
   </r>
   <r>
-    <s v="SK14 8GP"/>
-    <s v="Bungalow"/>
+    <x v="45"/>
     <x v="3"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="3"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-10-11T00:00:00"/>
     <d v="2022-01-14T00:00:00"/>
     <n v="272500"/>
     <n v="271500"/>
   </r>
   <r>
-    <s v="SK15 6YW"/>
-    <s v="Detatched"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Large"/>
+    <x v="46"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="2"/>
     <d v="2021-10-29T00:00:00"/>
     <d v="2022-02-24T00:00:00"/>
     <n v="389500"/>
     <n v="395000"/>
   </r>
   <r>
-    <s v="SK13 4DD"/>
-    <s v="Semi-detatched"/>
-    <x v="0"/>
+    <x v="47"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="2"/>
-    <s v="Medium"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <x v="0"/>
     <d v="2021-06-05T00:00:00"/>
     <d v="2022-01-22T00:00:00"/>
     <n v="348500"/>
     <n v="349500"/>
   </r>
   <r>
-    <s v="SK13 4RF"/>
-    <s v="Bungalow"/>
-    <x v="0"/>
-    <x v="2"/>
+    <x v="48"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
     <x v="1"/>
-    <x v="2"/>
-    <s v="Small"/>
     <d v="2022-01-31T00:00:00"/>
     <d v="2022-03-14T00:00:00"/>
     <n v="299950"/>
@@ -1237,12 +1272,74 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0DD47ADE-A6CD-A042-B38C-F60BC4296F8A}" name="PivotTable7" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:M35" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DFEA8CA5-EA12-8B43-8C93-480105B7BFFB}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0">
+      <items count="50">
+        <item x="12"/>
+        <item x="8"/>
+        <item x="41"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="47"/>
+        <item x="29"/>
+        <item x="6"/>
+        <item x="17"/>
+        <item x="48"/>
+        <item x="23"/>
+        <item x="36"/>
+        <item x="25"/>
+        <item x="43"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="39"/>
+        <item x="44"/>
+        <item x="30"/>
+        <item x="13"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="38"/>
+        <item x="22"/>
+        <item x="31"/>
+        <item x="18"/>
+        <item x="28"/>
+        <item x="40"/>
+        <item x="33"/>
+        <item x="19"/>
+        <item x="37"/>
+        <item x="7"/>
+        <item x="15"/>
+        <item x="24"/>
+        <item x="32"/>
+        <item x="3"/>
+        <item x="45"/>
+        <item x="10"/>
+        <item x="46"/>
+        <item x="27"/>
+        <item x="42"/>
+        <item x="16"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item x="11"/>
+        <item x="26"/>
+        <item x="21"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
       <items count="5">
         <item x="2"/>
         <item x="3"/>
@@ -1251,190 +1348,72 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="0"/>
         <item x="3"/>
-        <item x="2"/>
         <item x="1"/>
-        <item x="0"/>
-        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="2">
+    <pivotField name="Urban" axis="axisRow" showAll="0">
+      <items count="3">
         <item x="0"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="3">
-    <field x="3"/>
-    <field x="5"/>
-    <field x="4"/>
+  <rowFields count="2">
+    <field x="12"/>
+    <field x="2"/>
   </rowFields>
-  <rowItems count="29">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
     <i r="1">
       <x/>
     </i>
-    <i r="2">
-      <x/>
+    <i r="1">
+      <x v="1"/>
     </i>
     <i>
       <x v="1"/>
     </i>
     <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i>
       <x v="2"/>
     </i>
     <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i>
       <x v="3"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="3">
+  <colFields count="1">
     <field x="-2"/>
-    <field x="13"/>
-    <field x="2"/>
   </colFields>
-  <colItems count="12">
+  <colItems count="2">
     <i>
-      <x/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i r="2" i="1">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1" i="1">
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Sum of Field1" fld="11" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total Rooms" fld="12" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total Rooms" fld="11" baseField="0" baseItem="0"/>
+    <dataField name="Count of Garden Size" fld="6" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1744,1279 +1723,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD853B3-6D11-B64C-BF8E-76DCDA3197BF}">
-  <dimension ref="A3:M35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3353310F-EDD5-674D-A1C1-DC5FDF5D5B79}">
+  <dimension ref="A3:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="14">
+        <v>203</v>
+      </c>
+      <c r="C4" s="14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="14">
+        <v>148</v>
+      </c>
+      <c r="C5" s="14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="14">
+        <v>55</v>
+      </c>
+      <c r="C6" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L4" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" s="14">
+        <v>157</v>
+      </c>
+      <c r="C7" s="14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E6" t="s">
+      <c r="B8" s="14">
+        <v>145</v>
+      </c>
+      <c r="C8" s="14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
-        <v>1</v>
-      </c>
-      <c r="B7" s="15">
-        <v>0</v>
-      </c>
-      <c r="C7" s="15">
-        <v>0</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0</v>
-      </c>
-      <c r="E7" s="15">
-        <v>0</v>
-      </c>
-      <c r="F7" s="15">
-        <v>0</v>
-      </c>
-      <c r="G7" s="15">
-        <v>0</v>
-      </c>
-      <c r="H7" s="15">
-        <v>0</v>
-      </c>
-      <c r="I7" s="15">
-        <v>3</v>
-      </c>
-      <c r="J7" s="15">
-        <v>0</v>
-      </c>
-      <c r="K7" s="15">
-        <v>3</v>
-      </c>
-      <c r="L7" s="15">
-        <v>0</v>
-      </c>
-      <c r="M7" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
-        <v>1</v>
-      </c>
-      <c r="B8" s="15">
-        <v>0</v>
-      </c>
-      <c r="C8" s="15">
-        <v>0</v>
-      </c>
-      <c r="D8" s="15">
-        <v>0</v>
-      </c>
-      <c r="E8" s="15">
-        <v>0</v>
-      </c>
-      <c r="F8" s="15">
-        <v>0</v>
-      </c>
-      <c r="G8" s="15">
-        <v>0</v>
-      </c>
-      <c r="H8" s="15">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
-        <v>3</v>
-      </c>
-      <c r="J8" s="15">
-        <v>0</v>
-      </c>
-      <c r="K8" s="15">
-        <v>3</v>
-      </c>
-      <c r="L8" s="15">
-        <v>0</v>
-      </c>
-      <c r="M8" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="14">
-        <v>1</v>
-      </c>
-      <c r="B9" s="15">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15">
-        <v>0</v>
-      </c>
-      <c r="D9" s="15">
-        <v>0</v>
-      </c>
-      <c r="E9" s="15">
-        <v>0</v>
-      </c>
-      <c r="F9" s="15">
-        <v>0</v>
-      </c>
-      <c r="G9" s="15">
-        <v>0</v>
-      </c>
-      <c r="H9" s="15">
-        <v>0</v>
-      </c>
-      <c r="I9" s="15">
-        <v>3</v>
-      </c>
-      <c r="J9" s="15">
-        <v>0</v>
-      </c>
-      <c r="K9" s="15">
-        <v>3</v>
-      </c>
-      <c r="L9" s="15">
-        <v>0</v>
-      </c>
-      <c r="M9" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
-        <v>2</v>
-      </c>
-      <c r="B10" s="15">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15">
-        <v>0</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0</v>
-      </c>
-      <c r="E10" s="15">
-        <v>0</v>
-      </c>
-      <c r="F10" s="15">
-        <v>0</v>
-      </c>
-      <c r="G10" s="15">
-        <v>25</v>
-      </c>
-      <c r="H10" s="15">
-        <v>9</v>
-      </c>
-      <c r="I10" s="15">
-        <v>31</v>
-      </c>
-      <c r="J10" s="15">
-        <v>0</v>
-      </c>
-      <c r="K10" s="15">
-        <v>65</v>
-      </c>
-      <c r="L10" s="15">
-        <v>0</v>
-      </c>
-      <c r="M10" s="15">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
-        <v>1</v>
-      </c>
-      <c r="B11" s="15">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15">
-        <v>0</v>
-      </c>
-      <c r="D11" s="15">
-        <v>0</v>
-      </c>
-      <c r="E11" s="15">
-        <v>0</v>
-      </c>
-      <c r="F11" s="15">
-        <v>0</v>
-      </c>
-      <c r="G11" s="15">
-        <v>8</v>
-      </c>
-      <c r="H11" s="15">
-        <v>9</v>
-      </c>
-      <c r="I11" s="15">
-        <v>20</v>
-      </c>
-      <c r="J11" s="15">
-        <v>0</v>
-      </c>
-      <c r="K11" s="15">
-        <v>37</v>
-      </c>
-      <c r="L11" s="15">
-        <v>0</v>
-      </c>
-      <c r="M11" s="15">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="14">
-        <v>1</v>
-      </c>
-      <c r="B12" s="15">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15">
-        <v>0</v>
-      </c>
-      <c r="D12" s="15">
-        <v>0</v>
-      </c>
-      <c r="E12" s="15">
-        <v>0</v>
-      </c>
-      <c r="F12" s="15">
-        <v>0</v>
-      </c>
-      <c r="G12" s="15">
-        <v>8</v>
-      </c>
-      <c r="H12" s="15">
-        <v>4</v>
-      </c>
-      <c r="I12" s="15">
-        <v>20</v>
-      </c>
-      <c r="J12" s="15">
-        <v>0</v>
-      </c>
-      <c r="K12" s="15">
-        <v>32</v>
-      </c>
-      <c r="L12" s="15">
-        <v>0</v>
-      </c>
-      <c r="M12" s="15">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="14">
-        <v>2</v>
-      </c>
-      <c r="B13" s="15">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15">
-        <v>0</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0</v>
-      </c>
-      <c r="E13" s="15">
-        <v>0</v>
-      </c>
-      <c r="F13" s="15">
-        <v>0</v>
-      </c>
-      <c r="G13" s="15">
-        <v>0</v>
-      </c>
-      <c r="H13" s="15">
-        <v>5</v>
-      </c>
-      <c r="I13" s="15">
-        <v>0</v>
-      </c>
-      <c r="J13" s="15">
-        <v>0</v>
-      </c>
-      <c r="K13" s="15">
-        <v>5</v>
-      </c>
-      <c r="L13" s="15">
-        <v>0</v>
-      </c>
-      <c r="M13" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
-        <v>2</v>
-      </c>
-      <c r="B14" s="15">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15">
-        <v>0</v>
-      </c>
-      <c r="D14" s="15">
-        <v>0</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0</v>
-      </c>
-      <c r="F14" s="15">
-        <v>0</v>
-      </c>
-      <c r="G14" s="15">
-        <v>17</v>
-      </c>
-      <c r="H14" s="15">
-        <v>0</v>
-      </c>
-      <c r="I14" s="15">
-        <v>11</v>
-      </c>
-      <c r="J14" s="15">
-        <v>0</v>
-      </c>
-      <c r="K14" s="15">
-        <v>28</v>
-      </c>
-      <c r="L14" s="15">
-        <v>0</v>
-      </c>
-      <c r="M14" s="15">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="14">
-        <v>1</v>
-      </c>
-      <c r="B15" s="15">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15">
-        <v>0</v>
-      </c>
-      <c r="D15" s="15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="15">
-        <v>0</v>
-      </c>
-      <c r="G15" s="15">
-        <v>5</v>
-      </c>
-      <c r="H15" s="15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="15">
-        <v>5</v>
-      </c>
-      <c r="J15" s="15">
-        <v>0</v>
-      </c>
-      <c r="K15" s="15">
-        <v>10</v>
-      </c>
-      <c r="L15" s="15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="14">
-        <v>2</v>
-      </c>
-      <c r="B16" s="15">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15">
-        <v>0</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0</v>
-      </c>
-      <c r="E16" s="15">
-        <v>0</v>
-      </c>
-      <c r="F16" s="15">
-        <v>0</v>
-      </c>
-      <c r="G16" s="15">
+      <c r="B9" s="14">
         <v>12</v>
       </c>
-      <c r="H16" s="15">
-        <v>0</v>
-      </c>
-      <c r="I16" s="15">
-        <v>6</v>
-      </c>
-      <c r="J16" s="15">
-        <v>0</v>
-      </c>
-      <c r="K16" s="15">
-        <v>18</v>
-      </c>
-      <c r="L16" s="15">
-        <v>0</v>
-      </c>
-      <c r="M16" s="15">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="12">
-        <v>3</v>
-      </c>
-      <c r="B17" s="15">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15">
-        <v>0</v>
-      </c>
-      <c r="D17" s="15">
-        <v>0</v>
-      </c>
-      <c r="E17" s="15">
-        <v>0</v>
-      </c>
-      <c r="F17" s="15">
-        <v>0</v>
-      </c>
-      <c r="G17" s="15">
-        <v>97</v>
-      </c>
-      <c r="H17" s="15">
-        <v>21</v>
-      </c>
-      <c r="I17" s="15">
-        <v>71</v>
-      </c>
-      <c r="J17" s="15">
-        <v>12</v>
-      </c>
-      <c r="K17" s="15">
-        <v>201</v>
-      </c>
-      <c r="L17" s="15">
-        <v>0</v>
-      </c>
-      <c r="M17" s="15">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="13">
-        <v>1</v>
-      </c>
-      <c r="B18" s="15">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15">
-        <v>0</v>
-      </c>
-      <c r="D18" s="15">
-        <v>0</v>
-      </c>
-      <c r="E18" s="15">
-        <v>0</v>
-      </c>
-      <c r="F18" s="15">
-        <v>0</v>
-      </c>
-      <c r="G18" s="15">
-        <v>6</v>
-      </c>
-      <c r="H18" s="15">
-        <v>0</v>
-      </c>
-      <c r="I18" s="15">
-        <v>12</v>
-      </c>
-      <c r="J18" s="15">
-        <v>0</v>
-      </c>
-      <c r="K18" s="15">
-        <v>18</v>
-      </c>
-      <c r="L18" s="15">
-        <v>0</v>
-      </c>
-      <c r="M18" s="15">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="14">
-        <v>2</v>
-      </c>
-      <c r="B19" s="15">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15">
-        <v>0</v>
-      </c>
-      <c r="D19" s="15">
-        <v>0</v>
-      </c>
-      <c r="E19" s="15">
-        <v>0</v>
-      </c>
-      <c r="F19" s="15">
-        <v>0</v>
-      </c>
-      <c r="G19" s="15">
-        <v>6</v>
-      </c>
-      <c r="H19" s="15">
-        <v>0</v>
-      </c>
-      <c r="I19" s="15">
-        <v>12</v>
-      </c>
-      <c r="J19" s="15">
-        <v>0</v>
-      </c>
-      <c r="K19" s="15">
-        <v>18</v>
-      </c>
-      <c r="L19" s="15">
-        <v>0</v>
-      </c>
-      <c r="M19" s="15">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="13">
-        <v>2</v>
-      </c>
-      <c r="B20" s="15">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15">
-        <v>0</v>
-      </c>
-      <c r="D20" s="15">
-        <v>0</v>
-      </c>
-      <c r="E20" s="15">
-        <v>0</v>
-      </c>
-      <c r="F20" s="15">
-        <v>0</v>
-      </c>
-      <c r="G20" s="15">
-        <v>91</v>
-      </c>
-      <c r="H20" s="15">
-        <v>21</v>
-      </c>
-      <c r="I20" s="15">
-        <v>59</v>
-      </c>
-      <c r="J20" s="15">
-        <v>12</v>
-      </c>
-      <c r="K20" s="15">
-        <v>183</v>
-      </c>
-      <c r="L20" s="15">
-        <v>0</v>
-      </c>
-      <c r="M20" s="15">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="14">
-        <v>1</v>
-      </c>
-      <c r="B21" s="15">
-        <v>0</v>
-      </c>
-      <c r="C21" s="15">
-        <v>0</v>
-      </c>
-      <c r="D21" s="15">
-        <v>0</v>
-      </c>
-      <c r="E21" s="15">
-        <v>0</v>
-      </c>
-      <c r="F21" s="15">
-        <v>0</v>
-      </c>
-      <c r="G21" s="15">
-        <v>0</v>
-      </c>
-      <c r="H21" s="15">
-        <v>0</v>
-      </c>
-      <c r="I21" s="15">
-        <v>24</v>
-      </c>
-      <c r="J21" s="15">
-        <v>12</v>
-      </c>
-      <c r="K21" s="15">
-        <v>36</v>
-      </c>
-      <c r="L21" s="15">
-        <v>0</v>
-      </c>
-      <c r="M21" s="15">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="14">
-        <v>2</v>
-      </c>
-      <c r="B22" s="15">
-        <v>0</v>
-      </c>
-      <c r="C22" s="15">
-        <v>0</v>
-      </c>
-      <c r="D22" s="15">
-        <v>0</v>
-      </c>
-      <c r="E22" s="15">
-        <v>0</v>
-      </c>
-      <c r="F22" s="15">
-        <v>0</v>
-      </c>
-      <c r="G22" s="15">
-        <v>91</v>
-      </c>
-      <c r="H22" s="15">
-        <v>21</v>
-      </c>
-      <c r="I22" s="15">
-        <v>35</v>
-      </c>
-      <c r="J22" s="15">
-        <v>0</v>
-      </c>
-      <c r="K22" s="15">
-        <v>147</v>
-      </c>
-      <c r="L22" s="15">
-        <v>0</v>
-      </c>
-      <c r="M22" s="15">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="12">
-        <v>4</v>
-      </c>
-      <c r="B23" s="15">
-        <v>0</v>
-      </c>
-      <c r="C23" s="15">
-        <v>0</v>
-      </c>
-      <c r="D23" s="15">
-        <v>0</v>
-      </c>
-      <c r="E23" s="15">
-        <v>0</v>
-      </c>
-      <c r="F23" s="15">
-        <v>0</v>
-      </c>
-      <c r="G23" s="15">
-        <v>16</v>
-      </c>
-      <c r="H23" s="15">
-        <v>25</v>
-      </c>
-      <c r="I23" s="15">
-        <v>40</v>
-      </c>
-      <c r="J23" s="15">
-        <v>0</v>
-      </c>
-      <c r="K23" s="15">
-        <v>81</v>
-      </c>
-      <c r="L23" s="15">
-        <v>0</v>
-      </c>
-      <c r="M23" s="15">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
-        <v>1</v>
-      </c>
-      <c r="B24" s="15">
-        <v>0</v>
-      </c>
-      <c r="C24" s="15">
-        <v>0</v>
-      </c>
-      <c r="D24" s="15">
-        <v>0</v>
-      </c>
-      <c r="E24" s="15">
-        <v>0</v>
-      </c>
-      <c r="F24" s="15">
-        <v>0</v>
-      </c>
-      <c r="G24" s="15">
-        <v>0</v>
-      </c>
-      <c r="H24" s="15">
-        <v>0</v>
-      </c>
-      <c r="I24" s="15">
-        <v>7</v>
-      </c>
-      <c r="J24" s="15">
-        <v>0</v>
-      </c>
-      <c r="K24" s="15">
-        <v>7</v>
-      </c>
-      <c r="L24" s="15">
-        <v>0</v>
-      </c>
-      <c r="M24" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="14">
-        <v>2</v>
-      </c>
-      <c r="B25" s="15">
-        <v>0</v>
-      </c>
-      <c r="C25" s="15">
-        <v>0</v>
-      </c>
-      <c r="D25" s="15">
-        <v>0</v>
-      </c>
-      <c r="E25" s="15">
-        <v>0</v>
-      </c>
-      <c r="F25" s="15">
-        <v>0</v>
-      </c>
-      <c r="G25" s="15">
-        <v>0</v>
-      </c>
-      <c r="H25" s="15">
-        <v>0</v>
-      </c>
-      <c r="I25" s="15">
-        <v>7</v>
-      </c>
-      <c r="J25" s="15">
-        <v>0</v>
-      </c>
-      <c r="K25" s="15">
-        <v>7</v>
-      </c>
-      <c r="L25" s="15">
-        <v>0</v>
-      </c>
-      <c r="M25" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="13">
-        <v>2</v>
-      </c>
-      <c r="B26" s="15">
-        <v>0</v>
-      </c>
-      <c r="C26" s="15">
-        <v>0</v>
-      </c>
-      <c r="D26" s="15">
-        <v>0</v>
-      </c>
-      <c r="E26" s="15">
-        <v>0</v>
-      </c>
-      <c r="F26" s="15">
-        <v>0</v>
-      </c>
-      <c r="G26" s="15">
-        <v>16</v>
-      </c>
-      <c r="H26" s="15">
-        <v>16</v>
-      </c>
-      <c r="I26" s="15">
-        <v>24</v>
-      </c>
-      <c r="J26" s="15">
-        <v>0</v>
-      </c>
-      <c r="K26" s="15">
+      <c r="C9" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="14">
+        <v>360</v>
+      </c>
+      <c r="C10" s="14">
         <v>56</v>
-      </c>
-      <c r="L26" s="15">
-        <v>0</v>
-      </c>
-      <c r="M26" s="15">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="14">
-        <v>1</v>
-      </c>
-      <c r="B27" s="15">
-        <v>0</v>
-      </c>
-      <c r="C27" s="15">
-        <v>0</v>
-      </c>
-      <c r="D27" s="15">
-        <v>0</v>
-      </c>
-      <c r="E27" s="15">
-        <v>0</v>
-      </c>
-      <c r="F27" s="15">
-        <v>0</v>
-      </c>
-      <c r="G27" s="15">
-        <v>0</v>
-      </c>
-      <c r="H27" s="15">
-        <v>0</v>
-      </c>
-      <c r="I27" s="15">
-        <v>7</v>
-      </c>
-      <c r="J27" s="15">
-        <v>0</v>
-      </c>
-      <c r="K27" s="15">
-        <v>7</v>
-      </c>
-      <c r="L27" s="15">
-        <v>0</v>
-      </c>
-      <c r="M27" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="14">
-        <v>2</v>
-      </c>
-      <c r="B28" s="15">
-        <v>0</v>
-      </c>
-      <c r="C28" s="15">
-        <v>0</v>
-      </c>
-      <c r="D28" s="15">
-        <v>0</v>
-      </c>
-      <c r="E28" s="15">
-        <v>0</v>
-      </c>
-      <c r="F28" s="15">
-        <v>0</v>
-      </c>
-      <c r="G28" s="15">
-        <v>16</v>
-      </c>
-      <c r="H28" s="15">
-        <v>16</v>
-      </c>
-      <c r="I28" s="15">
-        <v>8</v>
-      </c>
-      <c r="J28" s="15">
-        <v>0</v>
-      </c>
-      <c r="K28" s="15">
-        <v>40</v>
-      </c>
-      <c r="L28" s="15">
-        <v>0</v>
-      </c>
-      <c r="M28" s="15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="14">
-        <v>3</v>
-      </c>
-      <c r="B29" s="15">
-        <v>0</v>
-      </c>
-      <c r="C29" s="15">
-        <v>0</v>
-      </c>
-      <c r="D29" s="15">
-        <v>0</v>
-      </c>
-      <c r="E29" s="15">
-        <v>0</v>
-      </c>
-      <c r="F29" s="15">
-        <v>0</v>
-      </c>
-      <c r="G29" s="15">
-        <v>0</v>
-      </c>
-      <c r="H29" s="15">
-        <v>0</v>
-      </c>
-      <c r="I29" s="15">
-        <v>9</v>
-      </c>
-      <c r="J29" s="15">
-        <v>0</v>
-      </c>
-      <c r="K29" s="15">
-        <v>9</v>
-      </c>
-      <c r="L29" s="15">
-        <v>0</v>
-      </c>
-      <c r="M29" s="15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="13">
-        <v>3</v>
-      </c>
-      <c r="B30" s="15">
-        <v>0</v>
-      </c>
-      <c r="C30" s="15">
-        <v>0</v>
-      </c>
-      <c r="D30" s="15">
-        <v>0</v>
-      </c>
-      <c r="E30" s="15">
-        <v>0</v>
-      </c>
-      <c r="F30" s="15">
-        <v>0</v>
-      </c>
-      <c r="G30" s="15">
-        <v>0</v>
-      </c>
-      <c r="H30" s="15">
-        <v>9</v>
-      </c>
-      <c r="I30" s="15">
-        <v>9</v>
-      </c>
-      <c r="J30" s="15">
-        <v>0</v>
-      </c>
-      <c r="K30" s="15">
-        <v>18</v>
-      </c>
-      <c r="L30" s="15">
-        <v>0</v>
-      </c>
-      <c r="M30" s="15">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="14">
-        <v>2</v>
-      </c>
-      <c r="B31" s="15">
-        <v>0</v>
-      </c>
-      <c r="C31" s="15">
-        <v>0</v>
-      </c>
-      <c r="D31" s="15">
-        <v>0</v>
-      </c>
-      <c r="E31" s="15">
-        <v>0</v>
-      </c>
-      <c r="F31" s="15">
-        <v>0</v>
-      </c>
-      <c r="G31" s="15">
-        <v>0</v>
-      </c>
-      <c r="H31" s="15">
-        <v>9</v>
-      </c>
-      <c r="I31" s="15">
-        <v>9</v>
-      </c>
-      <c r="J31" s="15">
-        <v>0</v>
-      </c>
-      <c r="K31" s="15">
-        <v>18</v>
-      </c>
-      <c r="L31" s="15">
-        <v>0</v>
-      </c>
-      <c r="M31" s="15">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="12">
-        <v>5</v>
-      </c>
-      <c r="B32" s="15">
-        <v>0</v>
-      </c>
-      <c r="C32" s="15">
-        <v>0</v>
-      </c>
-      <c r="D32" s="15">
-        <v>0</v>
-      </c>
-      <c r="E32" s="15">
-        <v>0</v>
-      </c>
-      <c r="F32" s="15">
-        <v>0</v>
-      </c>
-      <c r="G32" s="15">
-        <v>10</v>
-      </c>
-      <c r="H32" s="15">
-        <v>0</v>
-      </c>
-      <c r="I32" s="15">
-        <v>0</v>
-      </c>
-      <c r="J32" s="15">
-        <v>0</v>
-      </c>
-      <c r="K32" s="15">
-        <v>10</v>
-      </c>
-      <c r="L32" s="15">
-        <v>0</v>
-      </c>
-      <c r="M32" s="15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="13">
-        <v>3</v>
-      </c>
-      <c r="B33" s="15">
-        <v>0</v>
-      </c>
-      <c r="C33" s="15">
-        <v>0</v>
-      </c>
-      <c r="D33" s="15">
-        <v>0</v>
-      </c>
-      <c r="E33" s="15">
-        <v>0</v>
-      </c>
-      <c r="F33" s="15">
-        <v>0</v>
-      </c>
-      <c r="G33" s="15">
-        <v>10</v>
-      </c>
-      <c r="H33" s="15">
-        <v>0</v>
-      </c>
-      <c r="I33" s="15">
-        <v>0</v>
-      </c>
-      <c r="J33" s="15">
-        <v>0</v>
-      </c>
-      <c r="K33" s="15">
-        <v>10</v>
-      </c>
-      <c r="L33" s="15">
-        <v>0</v>
-      </c>
-      <c r="M33" s="15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="14">
-        <v>2</v>
-      </c>
-      <c r="B34" s="15">
-        <v>0</v>
-      </c>
-      <c r="C34" s="15">
-        <v>0</v>
-      </c>
-      <c r="D34" s="15">
-        <v>0</v>
-      </c>
-      <c r="E34" s="15">
-        <v>0</v>
-      </c>
-      <c r="F34" s="15">
-        <v>0</v>
-      </c>
-      <c r="G34" s="15">
-        <v>10</v>
-      </c>
-      <c r="H34" s="15">
-        <v>0</v>
-      </c>
-      <c r="I34" s="15">
-        <v>0</v>
-      </c>
-      <c r="J34" s="15">
-        <v>0</v>
-      </c>
-      <c r="K34" s="15">
-        <v>10</v>
-      </c>
-      <c r="L34" s="15">
-        <v>0</v>
-      </c>
-      <c r="M34" s="15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="15">
-        <v>0</v>
-      </c>
-      <c r="C35" s="15">
-        <v>0</v>
-      </c>
-      <c r="D35" s="15">
-        <v>0</v>
-      </c>
-      <c r="E35" s="15">
-        <v>0</v>
-      </c>
-      <c r="F35" s="15">
-        <v>0</v>
-      </c>
-      <c r="G35" s="15">
-        <v>148</v>
-      </c>
-      <c r="H35" s="15">
-        <v>55</v>
-      </c>
-      <c r="I35" s="15">
-        <v>145</v>
-      </c>
-      <c r="J35" s="15">
-        <v>12</v>
-      </c>
-      <c r="K35" s="15">
-        <v>360</v>
-      </c>
-      <c r="L35" s="15">
-        <v>0</v>
-      </c>
-      <c r="M35" s="15">
-        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>